<commit_message>
Added support for cross Browser testing Added annotation transformer Added retry analyzer Optimized Code
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/Data.xlsx
+++ b/src/test/resources/Data/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="runmanager" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -72,9 +72,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>failed</t>
   </si>
   <si>
@@ -84,7 +81,13 @@
     <t>yoloOldTest</t>
   </si>
   <si>
-    <t>5</t>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -408,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,10 +457,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -468,120 +471,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
+      <c r="F6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docker integration & Driverfactory creation
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/Data.xlsx
+++ b/src/test/resources/Data/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steav\Workspace2\YoutubeSeleniumFramework\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steav\Workspace2\SteaveSeleniumFramework\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
@@ -570,7 +570,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
@@ -590,7 +590,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>

</xml_diff>